<commit_message>
updated gantt chart, added legend
</commit_message>
<xml_diff>
--- a/docs/GantChart.xlsx
+++ b/docs/GantChart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mtabu\Documents\Temple University\Computational Engineering\Final_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99F900EC-4138-4547-A49E-1F3F6C0055A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B02356D-5023-4880-8D0B-291C17652759}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
   <si>
     <t>Task/Date</t>
   </si>
@@ -123,6 +123,21 @@
   <si>
     <t>Establish Timeline
 (Mason)</t>
+  </si>
+  <si>
+    <t>Green = Presentables</t>
+  </si>
+  <si>
+    <t>Blue = Backend</t>
+  </si>
+  <si>
+    <t>Orange = Critical Structure</t>
+  </si>
+  <si>
+    <t>Purple = Queries</t>
+  </si>
+  <si>
+    <t>Red = Frontend</t>
   </si>
 </sst>
 </file>
@@ -146,7 +161,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -177,6 +192,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="9">
     <border>
@@ -286,7 +307,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -305,7 +326,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
@@ -315,23 +335,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -339,9 +353,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -622,11 +644,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X71"/>
+  <dimension ref="A1:AC71"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="55" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A76" sqref="A76"/>
+      <selection pane="bottomLeft" activeCell="S17" sqref="S17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -644,135 +666,153 @@
     <col min="24" max="24" width="10.5546875" style="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A1" s="27"/>
-      <c r="B1" s="28" t="s">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A1" s="23"/>
+      <c r="B1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="30" t="s">
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="N1" s="28"/>
-      <c r="O1" s="28"/>
-      <c r="P1" s="28"/>
-      <c r="Q1" s="28"/>
-      <c r="R1" s="28"/>
-      <c r="S1" s="29"/>
-      <c r="T1" s="30" t="s">
+      <c r="N1" s="25"/>
+      <c r="O1" s="25"/>
+      <c r="P1" s="25"/>
+      <c r="Q1" s="25"/>
+      <c r="R1" s="25"/>
+      <c r="S1" s="26"/>
+      <c r="T1" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="U1" s="28"/>
-      <c r="V1" s="29"/>
-      <c r="W1" s="30" t="s">
+      <c r="U1" s="25"/>
+      <c r="V1" s="26"/>
+      <c r="W1" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="29"/>
-    </row>
-    <row r="2" spans="1:24" s="4" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="21" t="s">
+      <c r="X1" s="26"/>
+    </row>
+    <row r="2" spans="1:29" s="4" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="24">
+      <c r="B2" s="21">
         <v>45986</v>
       </c>
-      <c r="C2" s="24">
+      <c r="C2" s="21">
         <v>45987</v>
       </c>
-      <c r="D2" s="24">
+      <c r="D2" s="21">
         <v>45988</v>
       </c>
-      <c r="E2" s="24">
+      <c r="E2" s="21">
         <v>45989</v>
       </c>
-      <c r="F2" s="24">
+      <c r="F2" s="21">
         <v>45990</v>
       </c>
-      <c r="G2" s="24">
+      <c r="G2" s="21">
         <v>45991</v>
       </c>
-      <c r="H2" s="24">
+      <c r="H2" s="21">
         <v>45992</v>
       </c>
-      <c r="I2" s="24">
+      <c r="I2" s="21">
         <v>45993</v>
       </c>
-      <c r="J2" s="24">
+      <c r="J2" s="21">
         <v>45994</v>
       </c>
-      <c r="K2" s="24">
+      <c r="K2" s="21">
         <v>45995</v>
       </c>
-      <c r="L2" s="25">
+      <c r="L2" s="22">
         <v>45996</v>
       </c>
-      <c r="M2" s="24">
+      <c r="M2" s="21">
         <v>45997</v>
       </c>
-      <c r="N2" s="24">
+      <c r="N2" s="21">
         <v>45998</v>
       </c>
-      <c r="O2" s="24">
+      <c r="O2" s="21">
         <v>45999</v>
       </c>
-      <c r="P2" s="24">
+      <c r="P2" s="21">
         <v>46000</v>
       </c>
-      <c r="Q2" s="24">
+      <c r="Q2" s="21">
         <v>46001</v>
       </c>
-      <c r="R2" s="24">
+      <c r="R2" s="21">
         <v>46002</v>
       </c>
-      <c r="S2" s="25">
+      <c r="S2" s="22">
         <v>46003</v>
       </c>
-      <c r="T2" s="26">
+      <c r="T2" s="21">
         <v>46004</v>
       </c>
-      <c r="U2" s="26">
+      <c r="U2" s="21">
         <v>46005</v>
       </c>
-      <c r="V2" s="25">
+      <c r="V2" s="22">
         <v>46006</v>
       </c>
-      <c r="W2" s="26">
+      <c r="W2" s="21">
         <v>46007</v>
       </c>
-      <c r="X2" s="25">
+      <c r="X2" s="22">
         <v>46008</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="23" t="s">
+    <row r="3" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="28" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="22"/>
+    <row r="4" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="27"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="3"/>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A5" s="22"/>
-    </row>
-    <row r="6" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="23" t="s">
+      <c r="Z4" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA4" s="29"/>
+      <c r="AB4" s="29"/>
+      <c r="AC4" s="29"/>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A5" s="27"/>
+      <c r="Z5" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA5" s="29"/>
+      <c r="AB5" s="29"/>
+      <c r="AC5" s="29"/>
+    </row>
+    <row r="6" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="28" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="22"/>
+      <c r="Z6" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA6" s="29"/>
+      <c r="AB6" s="29"/>
+      <c r="AC6" s="29"/>
+    </row>
+    <row r="7" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="27"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -784,53 +824,69 @@
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
       <c r="L7" s="13"/>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A8" s="22"/>
-    </row>
-    <row r="9" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="23" t="s">
+      <c r="Z7" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA7" s="29"/>
+      <c r="AB7" s="29"/>
+      <c r="AC7" s="29"/>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A8" s="27"/>
+      <c r="Z8" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA8" s="29"/>
+      <c r="AB8" s="29"/>
+      <c r="AC8" s="29"/>
+    </row>
+    <row r="9" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="28" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="22"/>
+      <c r="Z9" s="29"/>
+      <c r="AA9" s="29"/>
+      <c r="AB9" s="29"/>
+      <c r="AC9" s="29"/>
+    </row>
+    <row r="10" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="27"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
       <c r="D10" s="8"/>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A11" s="22"/>
-    </row>
-    <row r="12" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="23" t="s">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A11" s="27"/>
+    </row>
+    <row r="12" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="28" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="22"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="14"/>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A14" s="22"/>
-    </row>
-    <row r="15" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="23" t="s">
+    <row r="13" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="27"/>
+      <c r="B13" s="30"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="30"/>
+      <c r="I13" s="30"/>
+      <c r="J13" s="30"/>
+      <c r="K13" s="30"/>
+      <c r="L13" s="31"/>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A14" s="27"/>
+    </row>
+    <row r="15" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="28" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="22"/>
+    <row r="16" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="27"/>
       <c r="B16" s="10"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
@@ -839,15 +895,15 @@
       <c r="G16" s="11"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A17" s="22"/>
+      <c r="A17" s="27"/>
     </row>
     <row r="18" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="23" t="s">
+      <c r="A18" s="28" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="23"/>
+      <c r="A19" s="28"/>
       <c r="B19" s="10"/>
       <c r="C19" s="10"/>
       <c r="D19" s="10"/>
@@ -856,15 +912,15 @@
       <c r="G19" s="11"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A20" s="23"/>
+      <c r="A20" s="28"/>
     </row>
     <row r="21" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="23" t="s">
+      <c r="A21" s="28" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="23"/>
+      <c r="A22" s="28"/>
       <c r="H22" s="9"/>
       <c r="I22" s="10"/>
       <c r="J22" s="10"/>
@@ -873,15 +929,15 @@
       <c r="M22" s="11"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A23" s="23"/>
+      <c r="A23" s="28"/>
     </row>
     <row r="24" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="23" t="s">
+      <c r="A24" s="28" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="22"/>
+      <c r="A25" s="27"/>
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
@@ -893,30 +949,30 @@
       <c r="J25" s="8"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A26" s="22"/>
+      <c r="A26" s="27"/>
     </row>
     <row r="27" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="22" t="s">
+      <c r="A27" s="27" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="22"/>
+      <c r="A28" s="27"/>
       <c r="G28" s="9"/>
       <c r="H28" s="10"/>
       <c r="I28" s="10"/>
       <c r="J28" s="11"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A29" s="22"/>
+      <c r="A29" s="27"/>
     </row>
     <row r="30" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="23" t="s">
+      <c r="A30" s="28" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="31" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="23"/>
+      <c r="A31" s="28"/>
       <c r="B31" s="10"/>
       <c r="C31" s="10"/>
       <c r="D31" s="10"/>
@@ -929,121 +985,121 @@
       <c r="K31" s="11"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A32" s="23"/>
+      <c r="A32" s="28"/>
     </row>
     <row r="33" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="23" t="s">
+      <c r="A33" s="28" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="34" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="23"/>
-      <c r="H34" s="15"/>
-      <c r="I34" s="16"/>
-      <c r="J34" s="16"/>
-      <c r="K34" s="16"/>
-      <c r="L34" s="16"/>
-      <c r="M34" s="16"/>
-      <c r="N34" s="16"/>
-      <c r="O34" s="18"/>
+      <c r="A34" s="28"/>
+      <c r="H34" s="14"/>
+      <c r="I34" s="15"/>
+      <c r="J34" s="15"/>
+      <c r="K34" s="15"/>
+      <c r="L34" s="15"/>
+      <c r="M34" s="15"/>
+      <c r="N34" s="15"/>
+      <c r="O34" s="17"/>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A35" s="23"/>
+      <c r="A35" s="28"/>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A36" s="23" t="s">
+      <c r="A36" s="28" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A37" s="23"/>
+      <c r="A37" s="28"/>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A38" s="23"/>
+      <c r="A38" s="28"/>
     </row>
     <row r="39" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="23" t="s">
+      <c r="A39" s="28" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="40" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="23"/>
-      <c r="H40" s="15"/>
-      <c r="I40" s="16"/>
-      <c r="J40" s="16"/>
-      <c r="K40" s="16"/>
-      <c r="L40" s="16"/>
-      <c r="M40" s="16"/>
-      <c r="N40" s="16"/>
-      <c r="O40" s="18"/>
+      <c r="A40" s="28"/>
+      <c r="H40" s="14"/>
+      <c r="I40" s="15"/>
+      <c r="J40" s="15"/>
+      <c r="K40" s="15"/>
+      <c r="L40" s="15"/>
+      <c r="M40" s="15"/>
+      <c r="N40" s="15"/>
+      <c r="O40" s="17"/>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A41" s="23"/>
+      <c r="A41" s="28"/>
     </row>
     <row r="42" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="23" t="s">
+      <c r="A42" s="28" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="43" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="23"/>
-      <c r="E43" s="15"/>
-      <c r="F43" s="16"/>
-      <c r="G43" s="16"/>
-      <c r="H43" s="16"/>
-      <c r="I43" s="16"/>
-      <c r="J43" s="16"/>
-      <c r="K43" s="16"/>
-      <c r="L43" s="17"/>
+      <c r="A43" s="28"/>
+      <c r="E43" s="14"/>
+      <c r="F43" s="15"/>
+      <c r="G43" s="15"/>
+      <c r="H43" s="15"/>
+      <c r="I43" s="15"/>
+      <c r="J43" s="15"/>
+      <c r="K43" s="15"/>
+      <c r="L43" s="16"/>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A44" s="23"/>
+      <c r="A44" s="28"/>
     </row>
     <row r="45" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="23" t="s">
+      <c r="A45" s="28" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="46" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="23"/>
-      <c r="E46" s="15"/>
-      <c r="F46" s="16"/>
-      <c r="G46" s="16"/>
-      <c r="H46" s="16"/>
-      <c r="I46" s="16"/>
-      <c r="J46" s="16"/>
-      <c r="K46" s="16"/>
-      <c r="L46" s="17"/>
+      <c r="A46" s="28"/>
+      <c r="E46" s="14"/>
+      <c r="F46" s="15"/>
+      <c r="G46" s="15"/>
+      <c r="H46" s="15"/>
+      <c r="I46" s="15"/>
+      <c r="J46" s="15"/>
+      <c r="K46" s="15"/>
+      <c r="L46" s="16"/>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A47" s="23"/>
+      <c r="A47" s="28"/>
     </row>
     <row r="48" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="23" t="s">
+      <c r="A48" s="28" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="49" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="23"/>
-      <c r="H49" s="15"/>
-      <c r="I49" s="16"/>
-      <c r="J49" s="16"/>
-      <c r="K49" s="16"/>
-      <c r="L49" s="16"/>
-      <c r="M49" s="16"/>
-      <c r="N49" s="16"/>
-      <c r="O49" s="18"/>
+      <c r="A49" s="28"/>
+      <c r="H49" s="14"/>
+      <c r="I49" s="15"/>
+      <c r="J49" s="15"/>
+      <c r="K49" s="15"/>
+      <c r="L49" s="15"/>
+      <c r="M49" s="15"/>
+      <c r="N49" s="15"/>
+      <c r="O49" s="17"/>
     </row>
     <row r="50" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A50" s="23"/>
+      <c r="A50" s="28"/>
     </row>
     <row r="51" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="22" t="s">
+      <c r="A51" s="27" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="52" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="22"/>
+      <c r="A52" s="27"/>
       <c r="B52" s="10"/>
       <c r="C52" s="10"/>
       <c r="D52" s="10"/>
@@ -1052,15 +1108,15 @@
       <c r="G52" s="11"/>
     </row>
     <row r="53" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A53" s="22"/>
+      <c r="A53" s="27"/>
     </row>
     <row r="54" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="22" t="s">
+      <c r="A54" s="27" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="55" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="22"/>
+      <c r="A55" s="27"/>
       <c r="B55" s="10"/>
       <c r="C55" s="10"/>
       <c r="D55" s="10"/>
@@ -1069,15 +1125,15 @@
       <c r="G55" s="11"/>
     </row>
     <row r="56" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A56" s="22"/>
+      <c r="A56" s="27"/>
     </row>
     <row r="57" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="22" t="s">
+      <c r="A57" s="27" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="58" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="22"/>
+      <c r="A58" s="27"/>
       <c r="B58" s="10"/>
       <c r="C58" s="10"/>
       <c r="D58" s="10"/>
@@ -1086,15 +1142,15 @@
       <c r="G58" s="11"/>
     </row>
     <row r="59" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A59" s="22"/>
+      <c r="A59" s="27"/>
     </row>
     <row r="60" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="22" t="s">
+      <c r="A60" s="27" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="61" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="22"/>
+      <c r="A61" s="27"/>
       <c r="K61" s="6"/>
       <c r="L61" s="7"/>
       <c r="M61" s="7"/>
@@ -1103,19 +1159,19 @@
       <c r="P61" s="7"/>
       <c r="Q61" s="7"/>
       <c r="R61" s="7"/>
-      <c r="S61" s="19"/>
+      <c r="S61" s="18"/>
     </row>
     <row r="62" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A62" s="22"/>
+      <c r="A62" s="27"/>
     </row>
     <row r="63" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="22" t="s">
+      <c r="A63" s="27" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="64" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="22"/>
-      <c r="M64" s="20"/>
+      <c r="A64" s="27"/>
+      <c r="M64" s="19"/>
       <c r="N64" s="2"/>
       <c r="O64" s="2"/>
       <c r="P64" s="2"/>
@@ -1129,44 +1185,45 @@
       <c r="X64" s="13"/>
     </row>
     <row r="65" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A65" s="22"/>
+      <c r="A65" s="27"/>
     </row>
     <row r="66" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="22" t="s">
+      <c r="A66" s="27" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="67" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A67" s="22"/>
+      <c r="A67" s="27"/>
       <c r="P67" s="1"/>
       <c r="Q67" s="2"/>
       <c r="R67" s="2"/>
       <c r="S67" s="13"/>
     </row>
     <row r="68" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A68" s="22"/>
+      <c r="A68" s="27"/>
     </row>
     <row r="69" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A69" s="22" t="s">
+      <c r="A69" s="27" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="70" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A70" s="22"/>
+      <c r="A70" s="27"/>
       <c r="T70" s="2"/>
       <c r="U70" s="2"/>
       <c r="V70" s="13"/>
     </row>
     <row r="71" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A71" s="22"/>
+      <c r="A71" s="27"/>
     </row>
   </sheetData>
-  <mergeCells count="27">
-    <mergeCell ref="M1:S1"/>
-    <mergeCell ref="T1:V1"/>
-    <mergeCell ref="W1:X1"/>
-    <mergeCell ref="A57:A59"/>
-    <mergeCell ref="A60:A62"/>
+  <mergeCells count="33">
+    <mergeCell ref="Z9:AC9"/>
+    <mergeCell ref="Z4:AC4"/>
+    <mergeCell ref="Z5:AC5"/>
+    <mergeCell ref="Z6:AC6"/>
+    <mergeCell ref="Z7:AC7"/>
+    <mergeCell ref="Z8:AC8"/>
     <mergeCell ref="A63:A65"/>
     <mergeCell ref="A66:A68"/>
     <mergeCell ref="A69:A71"/>
@@ -1183,6 +1240,11 @@
     <mergeCell ref="A33:A35"/>
     <mergeCell ref="A36:A38"/>
     <mergeCell ref="A39:A41"/>
+    <mergeCell ref="M1:S1"/>
+    <mergeCell ref="T1:V1"/>
+    <mergeCell ref="W1:X1"/>
+    <mergeCell ref="A57:A59"/>
+    <mergeCell ref="A60:A62"/>
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="A9:A11"/>

</xml_diff>

<commit_message>
claimed implementation of queue (priority queue)
</commit_message>
<xml_diff>
--- a/docs/GantChart.xlsx
+++ b/docs/GantChart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mtabu\Documents\Temple University\Computational Engineering\Final_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B02356D-5023-4880-8D0B-291C17652759}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0295CB33-4EBF-4166-A2EF-17708C85446C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -94,9 +94,6 @@
     <t>Design and Implement Sort #2</t>
   </si>
   <si>
-    <t>Queue</t>
-  </si>
-  <si>
     <t>Heap</t>
   </si>
   <si>
@@ -138,6 +135,10 @@
   </si>
   <si>
     <t>Red = Frontend</t>
+  </si>
+  <si>
+    <t>Queue
+(Mason)</t>
   </si>
 </sst>
 </file>
@@ -647,8 +648,8 @@
   <dimension ref="A1:AC71"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="55" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S17" sqref="S17"/>
+      <pane ySplit="2" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D66" sqref="D66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -682,7 +683,7 @@
       <c r="K1" s="25"/>
       <c r="L1" s="26"/>
       <c r="M1" s="24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N1" s="25"/>
       <c r="O1" s="25"/>
@@ -691,12 +692,12 @@
       <c r="R1" s="25"/>
       <c r="S1" s="26"/>
       <c r="T1" s="24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="U1" s="25"/>
       <c r="V1" s="26"/>
       <c r="W1" s="24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="X1" s="26"/>
     </row>
@@ -776,7 +777,7 @@
     </row>
     <row r="3" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="28" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -785,7 +786,7 @@
       <c r="C4" s="2"/>
       <c r="D4" s="3"/>
       <c r="Z4" s="29" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AA4" s="29"/>
       <c r="AB4" s="29"/>
@@ -794,7 +795,7 @@
     <row r="5" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A5" s="27"/>
       <c r="Z5" s="29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AA5" s="29"/>
       <c r="AB5" s="29"/>
@@ -805,7 +806,7 @@
         <v>5</v>
       </c>
       <c r="Z6" s="29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AA6" s="29"/>
       <c r="AB6" s="29"/>
@@ -825,7 +826,7 @@
       <c r="K7" s="2"/>
       <c r="L7" s="13"/>
       <c r="Z7" s="29" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="AA7" s="29"/>
       <c r="AB7" s="29"/>
@@ -834,7 +835,7 @@
     <row r="8" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A8" s="27"/>
       <c r="Z8" s="29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AA8" s="29"/>
       <c r="AB8" s="29"/>
@@ -1094,8 +1095,8 @@
       <c r="A50" s="28"/>
     </row>
     <row r="51" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="27" t="s">
-        <v>17</v>
+      <c r="A51" s="28" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="52" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1112,7 +1113,7 @@
     </row>
     <row r="54" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" s="27" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="55" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1129,7 +1130,7 @@
     </row>
     <row r="57" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="27" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="58" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1146,7 +1147,7 @@
     </row>
     <row r="60" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A60" s="27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="61" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1166,7 +1167,7 @@
     </row>
     <row r="63" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A63" s="27" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="64" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1189,7 +1190,7 @@
     </row>
     <row r="66" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A66" s="27" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="67" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1204,7 +1205,7 @@
     </row>
     <row r="69" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A69" s="27" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="70" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Claimed responsibility for implementing heap
</commit_message>
<xml_diff>
--- a/docs/GantChart.xlsx
+++ b/docs/GantChart.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mtabu\Documents\Temple University\Computational Engineering\Final_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0295CB33-4EBF-4166-A2EF-17708C85446C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64D5CD1C-514B-41B1-854D-14886AF89433}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$X$71</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$X$74</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
   <si>
     <t>Task/Date</t>
   </si>
@@ -138,6 +138,10 @@
   </si>
   <si>
     <t>Queue
+(Mason)</t>
+  </si>
+  <si>
+    <t>Heap
 (Mason)</t>
   </si>
 </sst>
@@ -345,6 +349,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -355,16 +364,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -645,11 +649,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AC71"/>
+  <dimension ref="A1:AC74"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="55" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D66" sqref="D66"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E70" sqref="E70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -669,37 +673,37 @@
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A1" s="23"/>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="24" t="s">
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="25"/>
-      <c r="R1" s="25"/>
-      <c r="S1" s="26"/>
-      <c r="T1" s="24" t="s">
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="28"/>
+      <c r="Q1" s="28"/>
+      <c r="R1" s="28"/>
+      <c r="S1" s="29"/>
+      <c r="T1" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="U1" s="25"/>
-      <c r="V1" s="26"/>
-      <c r="W1" s="24" t="s">
+      <c r="U1" s="28"/>
+      <c r="V1" s="29"/>
+      <c r="W1" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="X1" s="26"/>
+      <c r="X1" s="29"/>
     </row>
     <row r="2" spans="1:29" s="4" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="20" t="s">
@@ -776,44 +780,44 @@
       </c>
     </row>
     <row r="3" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="30" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="27"/>
+      <c r="A4" s="26"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="3"/>
-      <c r="Z4" s="29" t="s">
+      <c r="Z4" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="AA4" s="29"/>
-      <c r="AB4" s="29"/>
-      <c r="AC4" s="29"/>
+      <c r="AA4" s="31"/>
+      <c r="AB4" s="31"/>
+      <c r="AC4" s="31"/>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A5" s="27"/>
-      <c r="Z5" s="29" t="s">
+      <c r="A5" s="26"/>
+      <c r="Z5" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="AA5" s="29"/>
-      <c r="AB5" s="29"/>
-      <c r="AC5" s="29"/>
+      <c r="AA5" s="31"/>
+      <c r="AB5" s="31"/>
+      <c r="AC5" s="31"/>
     </row>
     <row r="6" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="Z6" s="29" t="s">
+      <c r="Z6" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="AA6" s="29"/>
-      <c r="AB6" s="29"/>
-      <c r="AC6" s="29"/>
+      <c r="AA6" s="31"/>
+      <c r="AB6" s="31"/>
+      <c r="AC6" s="31"/>
     </row>
     <row r="7" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="27"/>
+      <c r="A7" s="26"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -825,69 +829,69 @@
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
       <c r="L7" s="13"/>
-      <c r="Z7" s="29" t="s">
+      <c r="Z7" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="AA7" s="29"/>
-      <c r="AB7" s="29"/>
-      <c r="AC7" s="29"/>
+      <c r="AA7" s="31"/>
+      <c r="AB7" s="31"/>
+      <c r="AC7" s="31"/>
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A8" s="27"/>
-      <c r="Z8" s="29" t="s">
+      <c r="A8" s="26"/>
+      <c r="Z8" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="AA8" s="29"/>
-      <c r="AB8" s="29"/>
-      <c r="AC8" s="29"/>
+      <c r="AA8" s="31"/>
+      <c r="AB8" s="31"/>
+      <c r="AC8" s="31"/>
     </row>
     <row r="9" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="28" t="s">
+      <c r="A9" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="Z9" s="29"/>
-      <c r="AA9" s="29"/>
-      <c r="AB9" s="29"/>
-      <c r="AC9" s="29"/>
+      <c r="Z9" s="31"/>
+      <c r="AA9" s="31"/>
+      <c r="AB9" s="31"/>
+      <c r="AC9" s="31"/>
     </row>
     <row r="10" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="27"/>
+      <c r="A10" s="26"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
       <c r="D10" s="8"/>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A11" s="27"/>
+      <c r="A11" s="26"/>
     </row>
     <row r="12" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="28" t="s">
+      <c r="A12" s="30" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="27"/>
-      <c r="B13" s="30"/>
-      <c r="C13" s="30"/>
-      <c r="D13" s="30"/>
-      <c r="E13" s="30"/>
-      <c r="F13" s="30"/>
-      <c r="G13" s="30"/>
-      <c r="H13" s="30"/>
-      <c r="I13" s="30"/>
-      <c r="J13" s="30"/>
-      <c r="K13" s="30"/>
-      <c r="L13" s="31"/>
+      <c r="A13" s="26"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="24"/>
+      <c r="K13" s="24"/>
+      <c r="L13" s="25"/>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A14" s="27"/>
+      <c r="A14" s="26"/>
     </row>
     <row r="15" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="28" t="s">
+      <c r="A15" s="30" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="27"/>
+      <c r="A16" s="26"/>
       <c r="B16" s="10"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
@@ -896,15 +900,15 @@
       <c r="G16" s="11"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A17" s="27"/>
+      <c r="A17" s="26"/>
     </row>
     <row r="18" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="28" t="s">
+      <c r="A18" s="30" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="28"/>
+      <c r="A19" s="30"/>
       <c r="B19" s="10"/>
       <c r="C19" s="10"/>
       <c r="D19" s="10"/>
@@ -913,15 +917,15 @@
       <c r="G19" s="11"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A20" s="28"/>
+      <c r="A20" s="30"/>
     </row>
     <row r="21" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="28" t="s">
+      <c r="A21" s="30" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="28"/>
+      <c r="A22" s="30"/>
       <c r="H22" s="9"/>
       <c r="I22" s="10"/>
       <c r="J22" s="10"/>
@@ -930,15 +934,15 @@
       <c r="M22" s="11"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A23" s="28"/>
+      <c r="A23" s="30"/>
     </row>
     <row r="24" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="28" t="s">
+      <c r="A24" s="30" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="27"/>
+      <c r="A25" s="26"/>
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
@@ -950,30 +954,30 @@
       <c r="J25" s="8"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A26" s="27"/>
+      <c r="A26" s="26"/>
     </row>
     <row r="27" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="27" t="s">
+      <c r="A27" s="26" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="27"/>
+      <c r="A28" s="26"/>
       <c r="G28" s="9"/>
       <c r="H28" s="10"/>
       <c r="I28" s="10"/>
       <c r="J28" s="11"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A29" s="27"/>
+      <c r="A29" s="26"/>
     </row>
     <row r="30" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="28" t="s">
+      <c r="A30" s="30" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="31" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="28"/>
+      <c r="A31" s="30"/>
       <c r="B31" s="10"/>
       <c r="C31" s="10"/>
       <c r="D31" s="10"/>
@@ -986,15 +990,15 @@
       <c r="K31" s="11"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A32" s="28"/>
+      <c r="A32" s="30"/>
     </row>
     <row r="33" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="28" t="s">
+      <c r="A33" s="30" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="34" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="28"/>
+      <c r="A34" s="30"/>
       <c r="H34" s="14"/>
       <c r="I34" s="15"/>
       <c r="J34" s="15"/>
@@ -1005,26 +1009,26 @@
       <c r="O34" s="17"/>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A35" s="28"/>
+      <c r="A35" s="30"/>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A36" s="28" t="s">
+      <c r="A36" s="30" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A37" s="28"/>
+      <c r="A37" s="30"/>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A38" s="28"/>
+      <c r="A38" s="30"/>
     </row>
     <row r="39" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="28" t="s">
+      <c r="A39" s="30" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="40" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="28"/>
+      <c r="A40" s="30"/>
       <c r="H40" s="14"/>
       <c r="I40" s="15"/>
       <c r="J40" s="15"/>
@@ -1035,15 +1039,15 @@
       <c r="O40" s="17"/>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A41" s="28"/>
+      <c r="A41" s="30"/>
     </row>
     <row r="42" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="28" t="s">
+      <c r="A42" s="30" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="43" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="28"/>
+      <c r="A43" s="30"/>
       <c r="E43" s="14"/>
       <c r="F43" s="15"/>
       <c r="G43" s="15"/>
@@ -1054,15 +1058,15 @@
       <c r="L43" s="16"/>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A44" s="28"/>
+      <c r="A44" s="30"/>
     </row>
     <row r="45" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="28" t="s">
+      <c r="A45" s="30" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="46" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="28"/>
+      <c r="A46" s="30"/>
       <c r="E46" s="14"/>
       <c r="F46" s="15"/>
       <c r="G46" s="15"/>
@@ -1073,15 +1077,15 @@
       <c r="L46" s="16"/>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A47" s="28"/>
+      <c r="A47" s="30"/>
     </row>
     <row r="48" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="28" t="s">
+      <c r="A48" s="30" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="49" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="28"/>
+      <c r="A49" s="30"/>
       <c r="H49" s="14"/>
       <c r="I49" s="15"/>
       <c r="J49" s="15"/>
@@ -1092,32 +1096,35 @@
       <c r="O49" s="17"/>
     </row>
     <row r="50" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A50" s="28"/>
+      <c r="A50" s="30"/>
     </row>
     <row r="51" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="28" t="s">
+      <c r="A51" s="30" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="52" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="27"/>
+      <c r="A52" s="26"/>
       <c r="B52" s="10"/>
       <c r="C52" s="10"/>
       <c r="D52" s="10"/>
       <c r="E52" s="10"/>
       <c r="F52" s="10"/>
-      <c r="G52" s="11"/>
+      <c r="G52" s="10"/>
+      <c r="H52" s="10"/>
+      <c r="I52" s="10"/>
+      <c r="J52" s="11"/>
     </row>
     <row r="53" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A53" s="27"/>
+      <c r="A53" s="26"/>
     </row>
     <row r="54" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="27" t="s">
+      <c r="A54" s="26" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="55" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="27"/>
+      <c r="A55" s="26"/>
       <c r="B55" s="10"/>
       <c r="C55" s="10"/>
       <c r="D55" s="10"/>
@@ -1126,15 +1133,15 @@
       <c r="G55" s="11"/>
     </row>
     <row r="56" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A56" s="27"/>
+      <c r="A56" s="26"/>
     </row>
     <row r="57" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="27" t="s">
+      <c r="A57" s="26" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="58" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="27"/>
+      <c r="A58" s="26"/>
       <c r="B58" s="10"/>
       <c r="C58" s="10"/>
       <c r="D58" s="10"/>
@@ -1143,15 +1150,15 @@
       <c r="G58" s="11"/>
     </row>
     <row r="59" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A59" s="27"/>
+      <c r="A59" s="26"/>
     </row>
     <row r="60" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="27" t="s">
+      <c r="A60" s="26" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="61" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="27"/>
+      <c r="A61" s="26"/>
       <c r="K61" s="6"/>
       <c r="L61" s="7"/>
       <c r="M61" s="7"/>
@@ -1163,15 +1170,15 @@
       <c r="S61" s="18"/>
     </row>
     <row r="62" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A62" s="27"/>
+      <c r="A62" s="26"/>
     </row>
     <row r="63" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="27" t="s">
+      <c r="A63" s="26" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="64" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="27"/>
+      <c r="A64" s="26"/>
       <c r="M64" s="19"/>
       <c r="N64" s="2"/>
       <c r="O64" s="2"/>
@@ -1186,54 +1193,62 @@
       <c r="X64" s="13"/>
     </row>
     <row r="65" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A65" s="27"/>
+      <c r="A65" s="26"/>
     </row>
     <row r="66" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="27" t="s">
+      <c r="A66" s="26" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="67" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A67" s="27"/>
+      <c r="A67" s="26"/>
       <c r="P67" s="1"/>
       <c r="Q67" s="2"/>
       <c r="R67" s="2"/>
       <c r="S67" s="13"/>
     </row>
     <row r="68" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A68" s="27"/>
+      <c r="A68" s="26"/>
     </row>
     <row r="69" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A69" s="27" t="s">
+      <c r="A69" s="26" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="70" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A70" s="27"/>
+      <c r="A70" s="26"/>
       <c r="T70" s="2"/>
       <c r="U70" s="2"/>
       <c r="V70" s="13"/>
     </row>
     <row r="71" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A71" s="27"/>
+      <c r="A71" s="26"/>
+    </row>
+    <row r="72" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A72" s="30" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="73" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A73" s="26"/>
+      <c r="B73" s="10"/>
+      <c r="C73" s="10"/>
+      <c r="D73" s="10"/>
+      <c r="E73" s="10"/>
+      <c r="F73" s="10"/>
+      <c r="G73" s="11"/>
+    </row>
+    <row r="74" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A74" s="26"/>
     </row>
   </sheetData>
-  <mergeCells count="33">
+  <mergeCells count="34">
     <mergeCell ref="Z9:AC9"/>
     <mergeCell ref="Z4:AC4"/>
     <mergeCell ref="Z5:AC5"/>
     <mergeCell ref="Z6:AC6"/>
     <mergeCell ref="Z7:AC7"/>
     <mergeCell ref="Z8:AC8"/>
-    <mergeCell ref="A63:A65"/>
-    <mergeCell ref="A66:A68"/>
-    <mergeCell ref="A69:A71"/>
-    <mergeCell ref="B1:L1"/>
-    <mergeCell ref="A42:A44"/>
-    <mergeCell ref="A45:A47"/>
-    <mergeCell ref="A48:A50"/>
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="A51:A53"/>
     <mergeCell ref="A54:A56"/>
     <mergeCell ref="A24:A26"/>
     <mergeCell ref="A27:A29"/>
@@ -1241,6 +1256,12 @@
     <mergeCell ref="A33:A35"/>
     <mergeCell ref="A36:A38"/>
     <mergeCell ref="A39:A41"/>
+    <mergeCell ref="A42:A44"/>
+    <mergeCell ref="A45:A47"/>
+    <mergeCell ref="A48:A50"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="A72:A74"/>
     <mergeCell ref="M1:S1"/>
     <mergeCell ref="T1:V1"/>
     <mergeCell ref="W1:X1"/>
@@ -1252,6 +1273,10 @@
     <mergeCell ref="A12:A14"/>
     <mergeCell ref="A15:A17"/>
     <mergeCell ref="A18:A20"/>
+    <mergeCell ref="A63:A65"/>
+    <mergeCell ref="A66:A68"/>
+    <mergeCell ref="A69:A71"/>
+    <mergeCell ref="B1:L1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="31" orientation="portrait" r:id="rId1"/>

</xml_diff>